<commit_message>
configurando crud personas de frank
</commit_message>
<xml_diff>
--- a/Asignaciones.xlsx
+++ b/Asignaciones.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\SENA\Tareas Danillo\BaseCrud_Trabajo colaborativo\gitflow_practica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\repo\gitflow_practica\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE11187F-2291-46F3-AE17-80B97588C610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="41">
   <si>
     <t>#</t>
   </si>
@@ -92,9 +93,6 @@
     <t>Actualizar Producto</t>
   </si>
   <si>
-    <t>TEAM:Donnovan,Daniel</t>
-  </si>
-  <si>
     <t>LIDER: Daniel Rojas</t>
   </si>
   <si>
@@ -126,12 +124,36 @@
   </si>
   <si>
     <t>f_eliminar_producto</t>
+  </si>
+  <si>
+    <t>TEAM:Donnovan,Daniel,Frank</t>
+  </si>
+  <si>
+    <t>frank</t>
+  </si>
+  <si>
+    <t>f_actualizar_persona</t>
+  </si>
+  <si>
+    <t>f_agregar_persona</t>
+  </si>
+  <si>
+    <t>f_eliminar_persona</t>
+  </si>
+  <si>
+    <t>f_menu_persona</t>
+  </si>
+  <si>
+    <t>f_consultar_producto</t>
+  </si>
+  <si>
+    <t>f_consultar_persona</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -174,7 +196,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,6 +224,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD0E0E3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -278,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -330,6 +358,21 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -615,11 +658,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -635,10 +678,10 @@
     <row r="1" spans="1:7" ht="15.75" customHeight="1" thickBot="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -695,7 +738,7 @@
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.25" customHeight="1" thickBot="1">
@@ -709,14 +752,14 @@
         <v>11</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" thickBot="1">
@@ -730,14 +773,14 @@
         <v>13</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" thickBot="1">
@@ -751,14 +794,14 @@
         <v>15</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="16.5" customHeight="1" thickBot="1">
@@ -769,17 +812,17 @@
         <v>16</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.25" customHeight="1" thickBot="1">
@@ -790,17 +833,17 @@
         <v>17</v>
       </c>
       <c r="C9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>25</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>26</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" thickBot="1">
@@ -811,17 +854,17 @@
         <v>18</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" thickBot="1">
@@ -832,17 +875,17 @@
         <v>19</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18.75" customHeight="1" thickBot="1">
@@ -853,17 +896,17 @@
         <v>20</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="18" customHeight="1" thickBot="1">
@@ -874,17 +917,17 @@
         <v>21</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="18" customHeight="1" thickBot="1">
@@ -895,17 +938,122 @@
         <v>17</v>
       </c>
       <c r="C14" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>30</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>31</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>9</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="21" thickBot="1">
+      <c r="A15" s="18">
+        <v>12</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="20"/>
+      <c r="G15" s="21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="21" thickBot="1">
+      <c r="A16" s="18">
+        <v>13</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="21" thickBot="1">
+      <c r="A17" s="18">
+        <v>14</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="20"/>
+      <c r="G17" s="21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="21" thickBot="1">
+      <c r="A18" s="18">
+        <v>15</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="20"/>
+      <c r="G18" s="21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="21" thickBot="1">
+      <c r="A19" s="18">
+        <v>16</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="22"/>
+      <c r="G19" s="21" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>